<commit_message>
Revert "increased test cases"
</commit_message>
<xml_diff>
--- a/local_testcases.xlsx
+++ b/local_testcases.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F46"/>
+  <dimension ref="A1:F59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,27 +456,29 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>TC001</t>
+          <t>TC_FILE_001</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Verify successful creation of a new empty document and saving it to a specified new file, including path and filename validations.</t>
+          <t>Verify user can successfully create a new empty document.</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Application is running.</t>
+          <t>Application is launched and no document is open.</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>1. Navigate to 'File' menu. 2. Select 'New Document'. 3. Verify an empty document is displayed. 4. Navigate to 'File' menu. 5. Select 'Save As'. 6. Choose a new valid file path and name (e.g., 'MyNewDoc.req', max allowed length filename, special allowed characters). 7. Click 'Save'. 8. (Negative) Repeat steps 4-5. 9. Attempt to save with invalid characters in the filename (e.g., '&lt;&gt;?*:|'). 10. Attempt to save to a non-existent directory. 11. Attempt to save to a read-only system directory (e.g., C:\Program Files). 12. During the 'Save As' dialog, click 'Cancel'.</t>
+          <t>1. Click 'File' -&gt; 'New Document'.
+2. Observe the application interface.
+3. Verify the document's initial state.</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>An empty document is displayed. The document is successfully saved to the specified new file without errors. The application title reflects the new file name. An error message is displayed for invalid filename characters. An error message is displayed for a non-existent directory. An error message is displayed for insufficient permissions/read-only location. The 'Save As' dialog closes without saving the document when 'Cancel' is clicked.</t>
+          <t>A new, untitled, empty document workspace is displayed, ready for content creation. The document contains a default root section or is completely empty, allowing immediate addition of content. No errors are shown, and the application remains responsive.</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -488,59 +490,65 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>TC002</t>
+          <t>TC_FILE_001_NEG_001</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Verify opening a valid existing document and saving changes by overwriting the file, including error handling for file locks.</t>
+          <t>Verify application handles creating a new document with an invalid name (if prompted for a name during creation).</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>A valid document file (e.g., 'ExistingDoc.req') exists on the file system. A read-only version of this file also exists ('ReadOnlyDoc.req').</t>
+          <t>Application is launched and no document is open. The 'New Document' workflow prompts for a document name.</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>1. Navigate to 'File' menu. 2. Select 'Open Document'. 3. Choose 'ExistingDoc.req' and click 'Open'. 4. Create a new requirement in the document. 5. Navigate to 'File' menu. 6. Select 'Save'. 7. (Negative) Open 'ReadOnlyDoc.req'. 8. Attempt to make changes. 9. Attempt to save 'ReadOnlyDoc.req'. 10. (Negative) Simulate another process locking 'ExistingDoc.req'. 11. Open 'ExistingDoc.req'. 12. Make changes. 13. Attempt to save. 14. During a save operation (if a prompt appears), click 'Cancel'.</t>
+          <t>1. Click 'File' -&gt; 'New Document'.
+2. When prompted for a name, enter an invalid name (e.g., empty string, string with restricted characters like '/', ':', '*', '?', '&lt;', '&gt;', '|').
+3. Attempt to confirm creation.</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>The 'ExistingDoc.req' is opened and its content is displayed correctly. The new requirement is added. The document is saved, overwriting 'ExistingDoc.req' successfully without any prompts for a new file name. For 'ReadOnlyDoc.req', changes are prevented or an error is displayed upon save attempt (e.g., 'File is read-only'). For a locked file, an error message is displayed indicating the file is in use or locked. The save operation is canceled, and the document remains in its modified state.</t>
+          <t>The application displays a clear error message (e.g., 'Invalid Document Name', 'Name cannot be empty', 'Contains forbidden characters') and prevents the creation of the document. The application remains stable.</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>High</t>
+          <t>Medium</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>TC003</t>
+          <t>TC_FILE_002</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Verify successful import of structured MS Word and MS Excel table of requirements, including handling of invalid/edge cases.</t>
+          <t>Verify application handles 'permission denied' error when saving a document to a restricted location.</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Application is running. Structured MS Word document ('Structured.docx'), MS Excel table of requirements ('Structured.xlsx'), an empty Word file ('Empty.docx'), a password-protected Excel file ('Protected.xlsx'), and a non-structured Word document ('NonStructured.docx') are available.</t>
+          <t>A new document is open with some content.
+User attempts to save to a read-only location (e.g., system directory, network share without write access).</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>1. Create a new empty document. 2. Navigate to 'File' menu. 3. Select 'Import' -&gt; 'MS Word Document'. 4. Choose 'Structured.docx' and click 'Import'. 5. Verify requirements are imported. 6. Repeat steps 2-4 for 'MS Excel Table' using 'Structured.xlsx'. 7. (Negative) Attempt to import 'Empty.docx'. 8. (Negative) Attempt to import 'Protected.xlsx'. 9. (Negative) Attempt to import 'NonStructured.docx' (e.g., a plain text document). 10. (Edge) Import a Word document with only a single heading or an Excel file with only header row. 11. (Edge) Import an extremely large structured document (e.g., 50MB, 1000+ requirements) and monitor performance. 12. During an import operation, click 'Cancel'.</t>
+          <t>1. Create a new document and add a requirement.
+2. Click 'File' -&gt; 'Save As'.
+3. Navigate to a folder where the user does not have write permissions.
+4. Attempt to save the document.</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>The Word document content is successfully imported, correctly parsing sections, headings, and requirement text. The Excel table data is imported, correctly mapping columns to requirement attributes. No parsing errors occur. An error/warning is displayed for empty files. An error is displayed for password-protected files. An error/warning is displayed for non-structured/unsupported formats. Edge case files are imported correctly, resulting in appropriate number of requirements/sections. Large document import completes within reasonable time without crashes. The import operation is aborted when 'Cancel' is clicked.</t>
+          <t>The application displays an explicit error message indicating 'Permission Denied', 'Access Denied', or 'Insufficient Write Privileges'. The document is NOT saved to that location, and the user is prompted to choose another location or cancel. Unsaved changes remain in the current document state. The application remains stable.</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -552,59 +560,63 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>TC004</t>
+          <t>TC_FILE_003</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Verify successful export of the displayed document view to HTML and requirements to CSV, including error handling.</t>
+          <t>Verify user can successfully import requirements from a valid MS Excel file.</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>An opened document containing requirements and sections is displayed. A read-only directory exists.</t>
+          <t>Application is launched and a new document is open.
+A valid MS Excel file containing requirements data (headings, levels, text, custom attributes, links) is available, adhering to the specified import format.</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>1. Navigate to 'File' menu. 2. Select 'Export' -&gt; 'HTML'. 3. Choose a destination path and file name (e.g., 'ExportedDoc.html'). 4. Click 'Save'. 5. Verify the generated HTML file. 6. Navigate to 'File' menu. 7. Select 'Export' -&gt; 'CSV'. 8. Choose a destination path and file name (e.g., 'ExportedReqs.csv'). 9. Click 'Save'. 10. Verify the generated CSV file. 11. (Negative) Attempt to export to a read-only directory. 12. (Edge) Export an empty document. 13. (Edge) Export a document with complex rich text (tables, images) in descriptions (for HTML export). 14. During an export operation, click 'Cancel'.</t>
+          <t>1. Click 'File' -&gt; 'Import' -&gt; 'MS Excel'.
+2. Select the valid Excel file and proceed with import, ensuring correct column mappings for all data types (text, numbers, booleans, dates, custom attributes).
+3. Confirm import and observe the document content.</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>An HTML file is generated and saved, accurately representing the displayed document view (sections, requirements, formatting). A CSV file is generated and saved, containing requirements data with correct column headers and values. Exported files are valid and open correctly in respective applications. An error message is displayed when attempting to export to a read-only location. Empty document exports produce an HTML file with only basic structure/headings, and an empty (or only headers) CSV. Complex rich text is accurately converted to HTML. The export operation is aborted when 'Cancel' is clicked.</t>
+          <t>Requirements from the Excel file are successfully imported into the document. Headings, hierarchical levels, requirement text, custom attribute values, and link definitions (if supported by import) are preserved and displayed accurately. No errors are displayed, and the import process completes within an acceptable time frame.</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>High</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>TC005</t>
+          <t>TC_FILE_003_NEG_001</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Verify the display of the table of contents for a multi-section document and focusing a section, including edge cases.</t>
+          <t>Verify application handles importing from a non-existent or inaccessible Excel file.</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>An opened document with multiple sections (e.g., Section 1, Section 1.1, Section 2), and a document with a deep hierarchy (e.g., Section 1.1.1.1).</t>
+          <t>Application is launched and a new document is open.</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>1. Ensure the Table of Contents pane is visible. 2. Observe the TOC structure for the multi-section document. 3. Click on a specific section (e.g., 'Section 1.1') in the TOC. 4. (Edge) Open the document with a deep hierarchy. 5. Click on the deepest nested section. 6. (Edge) Open a document with a very large number of top-level sections (e.g., 50+). 7. (Negative) Open a document with no sections (fresh new document).</t>
+          <t>1. Click 'File' -&gt; 'Import' -&gt; 'MS Excel'.
+2. Attempt to select or provide a path to an Excel file that does not exist or is currently locked/inaccessible (e.g., deleted, open exclusively by another process).</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>The Table of Contents pane accurately displays the document structure with hierarchical sections. Clicking on 'Section 1.1' causes the requirements table to scroll and focus on 'Section 1.1', making it visible and highlighted. For deep hierarchies, the TOC expands correctly, and navigation works. For many top-level sections, the TOC loads efficiently and remains usable. For a document with no sections, the TOC pane should be empty or display an appropriate message (e.g., 'No sections defined').</t>
+          <t>The application displays an error message (e.g., 'File not found', 'Access denied', 'File is in use') and prevents the import. The application remains stable.</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -616,59 +628,65 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>TC006</t>
+          <t>TC_FILE_003_NEG_002</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Verify requirements table displays all standard and custom columns correctly, including unique IDs and content, under various data conditions.</t>
+          <t>Verify application handles importing from a malformed or corrupted Excel file.</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>An opened document containing requirements with various populated fields (ID, Description, Discussion, Links, Custom attributes of different types) is displayed. Include a requirement with all fields populated to their maximum reasonable length.</t>
+          <t>Application is launched and a new document is open.
+A malformed (e.g., incorrect file extension, unreadable content) or corrupted Excel file is available.</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>1. Ensure all standard columns (ID, Description, Discussion, Links) are visible. 2. Create at least one custom attribute of each type (Enum, XHTML, Integer, String) and ensure their columns are visible. 3. Observe the displayed table content for a regular requirement. 4. Observe the displayed table content for the requirement with maximum reasonable length content in all fields.</t>
+          <t>1. Click 'File' -&gt; 'Import' -&gt; 'MS Excel'.
+2. Select the malformed/corrupted Excel file.
+3. Attempt to proceed with import.</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>All configured standard and custom columns are displayed. Unique requirement identifiers are correctly shown in the 'ID' column. Section numbers, headings, requirement text, and attachments are displayed in the 'Description' column, rendering rich text correctly. Comments appear in 'Discussion', and traceability links (grouped by type) appear in 'Links'. Custom attribute values are correctly displayed according to their type (e.g., Enum values, rich text for XHTML, numbers for Integer). For the max length content requirement, all data is displayed without truncation or corruption, and the UI handles overflow (e.g., scrollbars, ellipsis).</t>
+          <t>The application displays an error message indicating that the file is invalid or corrupted and cannot be parsed. The import process is halted, and no data is imported. The application remains stable.</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>High</t>
+          <t>Medium</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>TC007</t>
+          <t>TC_FILE_003_NEG_003</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Verify column width adjustment, reordering, and show/hide functionality, and persistence of these settings.</t>
+          <t>Verify application handles importing from an Excel file with incorrect or missing required column mappings.</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>An opened document with multiple columns displayed in the requirements table.</t>
+          <t>Application is launched and a new document is open.
+An Excel file is available where a mandatory column (e.g., 'ID' or 'Description') is missing, or a column is mapped to an incompatible data type.</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>1. Drag the border of a column header (e.g., 'Description') to change its width: first to a very narrow width, then to a very wide width. 2. Drag a column header (e.g., 'Links') to reorder it to the first position, then to the last position. 3. Use the column visibility settings to hide a column (e.g., 'Discussion'). 4. Use the column visibility settings to show the 'Discussion' column again. 5. (Negative) Attempt to hide the 'ID' column (as per TC023). 6. Close and restart the application. 7. Open the same document.</t>
+          <t>1. Click 'File' -&gt; 'Import' -&gt; 'MS Excel'.
+2. Select the Excel file.
+3. Attempt to proceed with import where column mappings are incorrect or mandatory columns are not mapped.</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>The column width adjusts as dragged, respecting minimum/maximum logical widths. Columns are successfully reordered to the new positions. The selected column hides and shows correctly without affecting other columns or table functionality. The 'ID' column cannot be hidden. Upon application restart and document re-opening, all column width, order, and visibility settings are persisted and restored correctly.</t>
+          <t>The application identifies the mapping issue (e.g., 'Missing required column', 'Invalid data type mapping for column X') and prompts the user to correct it or cancels the import. No partial or corrupted data is imported. The application remains stable.</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -680,59 +698,64 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>TC008</t>
+          <t>TC_FILE_003_EDGE_001</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Verify sorting requirements table columns in ascending and descending order, including edge cases and non-sortable columns.</t>
+          <t>Verify application handles importing from an empty Excel file (no data rows, only headers).</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>An opened document with requirements and values in sortable columns (e.g., ID, Custom Integer, Custom String, Custom Date/Time). Include columns with all identical values, and a column with mixed data types if allowed.</t>
+          <t>Application is launched and a new document is open.
+An Excel file containing only column headers and no data rows is available.</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>1. Click on the 'ID' column header to sort in ascending order. 2. Click on the 'ID' column header again to sort in descending order. 3. Repeat steps 1-2 for a custom attribute column (e.g., 'Priority' - Integer). 4. Repeat steps 1-2 for a Custom String column, verifying case-insensitive sorting (if applicable). 5. (Edge) Sort a column where all values are identical. 6. (Negative) Click on the 'Discussion' column header to attempt sorting. 7. (Negative) Click on the 'Links' column header to attempt sorting.</t>
+          <t>1. Click 'File' -&gt; 'Import' -&gt; 'MS Excel'.
+2. Select the empty Excel file and proceed with import.</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Requirements are sorted correctly by 'ID' in ascending order. Requirements are then sorted correctly by 'ID' in descending order. Custom attribute columns also sort correctly in both ascending and descending orders, respecting their data type. For columns with identical values, their relative order should remain stable (stable sort). Clicking on 'Discussion' or 'Links' column headers has no effect on sorting; requirements do not reorder, indicating sorting is not supported for these columns. The table remains stable after sorting.</t>
+          <t>The import process completes successfully, but no requirements are added to the document. The application might display a message like 'No data rows found' or simply show no new content. No errors are displayed, and the application remains stable.</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Low</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>TC009</t>
+          <t>TC_FILE_003_SEC_001</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Verify displaying detailed information for a selected requirement (Custom Attributes, Discussion, Links panes) and UI responsiveness.</t>
+          <t>Verify application handles importing an Excel file containing malicious macros or embedded scripts.</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>An opened document. A requirement with various custom attribute values, multiple comments, and various traceability links exists. Include a requirement with a very large number of comments (e.g., 100+), links (e.g., 50+), and custom attributes (e.g., 20+).</t>
+          <t>Application is launched and a new document is open.
+An Excel file containing known malicious macros, OLE objects with embedded scripts, or other security threats is available.</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>1. Select a requirement in the table. 2. Ensure the 'Custom Attributes' pane is visible. 3. Ensure the 'Discussion' pane is visible, then expand/collapse some comments. 4. Ensure the 'Links' pane is visible. 5. Select a requirement with minimal details (no custom attributes, no comments, no links). 6. Select the requirement with a very large number of comments/links/custom attributes.</t>
+          <t>1. Click 'File' -&gt; 'Import' -&gt; 'MS Excel'.
+2. Select the malicious Excel file.
+3. Attempt to proceed with import.</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>The 'Custom Attributes' pane displays all assigned custom attribute values for the selected requirement, showing appropriate widgets for each type. The 'Discussion' pane displays all comments, ordered by date/time, and comments expand/collapse correctly. The 'Links' pane displays traceability links, grouped by type and ordered by linked object ID, showing link directionality. The panes update instantly and correctly when a different requirement is selected, even for requirements with many associated details, without UI freezes or significant delays.</t>
+          <t>The application should safely handle the file, ideally detecting and stripping any malicious content or blocking the import. No scripts should be executed within the application context. The application remains stable and secure, with no compromise to its integrity or the user's system.</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -744,59 +767,64 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>TC010</t>
+          <t>TC_FILE_004</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Verify creation of a new requirement within an existing section and a newly created section, including edge cases.</t>
+          <t>Verify user can successfully export the current document view to HTML.</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>An opened document with at least one existing section. Document also contains no sections for testing initial creation.</t>
+          <t>A document with multiple sections, requirements (including rich text, custom attributes, links), and possibly images is open and displayed in the main view.</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>1. (Edge) Create a new empty document. 2. Use the 'Create Section' action (or equivalent) to add the very first section. 3. Select this new section. 4. Use the 'Create Requirement' action. 5. Verify the new requirement is placed under the selected section. 6. Select an existing section in a populated document. 7. Use the 'Create Requirement' action. 8. Verify the new requirement is placed under the selected section. 9. Use the 'Create Section' action to add another new section (e.g., nested under an existing one). 10. Select the newly created section. 11. Use the 'Create Requirement' action. 12. Verify the new requirement is placed under the newly created section. 13. Create a new requirement at the very end of the document.</t>
+          <t>1. Click 'File' -&gt; 'Export' -&gt; 'HTML'.
+2. Choose a valid save location and provide a valid filename.
+3. Confirm export.
+4. Open the generated HTML file in a standard web browser (e.g., Chrome, Firefox).</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>A new section is successfully created as the first item. A new requirement is successfully created and positioned correctly within the new section. A new requirement is successfully created and positioned correctly within the existing section. Another new section is created. Another new requirement is successfully created and positioned correctly within the newly created section. Unique IDs are assigned to all new requirements and sections, and numbering is updated correctly. The requirement at the end is added correctly.</t>
+          <t>An HTML file is successfully created at the specified location. The HTML file accurately displays the document's sections, headings, requirements, rich text formatting, and their visible attributes (ID, Description, custom attributes) as seen in the application's current view. Embedded images (if supported) are correctly displayed. The HTML structure is valid and renders consistently across different browsers.</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>High</t>
+          <t>Medium</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>TC011</t>
+          <t>TC_FILE_004_NEG_001</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Verify copying multiple selected requirements and moving a selected document section, including edge cases and negative scenarios.</t>
+          <t>Verify application handles exporting to a non-existent or inaccessible directory.</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>An opened document with at least two requirements and two sections. A deleted requirement and section also exist.</t>
+          <t>A document is open.</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>1. Select multiple active requirements (e.g., Req A and Req B). 2. Use the 'Copy' action. 3. Select a different section. 4. Use the 'Paste' action. 5. Verify new copies are created. 6. Select a document section (e.g., Section X) containing sub-sections and requirements. 7. Use the 'Move' action and choose a new location (e.g., after Section Y, or deeply nested). 8. Verify the section is moved. 9. (Negative) Select a deleted requirement. 10. Attempt to 'Copy' it. 11. (Negative) Select a deleted section. 12. Attempt to 'Move' it. 13. (Negative) Attempt to move a section to be its own child.</t>
+          <t>1. Click 'File' -&gt; 'Export' -&gt; 'HTML'.
+2. Attempt to choose a save location that does not exist or where the user lacks write permissions.
+3. Attempt to proceed with export.</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Multiple copies of the selected requirements are created in the target section, each with new unique IDs and retaining their original content (excluding comments, links, etc. if 'copy' implies fresh start). The selected document section (and all its contents) is successfully moved to the new location, retaining its requirements and sub-sections, and its numbering is updated if applicable. Copying/Moving deleted items should be disabled or result in an error message. Attempting to move a section to be its own child should be prevented with an error.</t>
+          <t>The application displays an error message (e.g., 'Directory not found', 'Permission denied', 'Invalid path') and prevents the export. The application remains stable.</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -808,27 +836,29 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>TC012</t>
+          <t>TC_FILE_004_SEC_001</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Verify marking a requirement as deleted, undeleting it, and permanently removing a deleted requirement/section.</t>
+          <t>Verify HTML export sanitizes user-entered content to prevent XSS vulnerabilities in the exported file.</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>An opened document with at least one requirement and one section (with sub-requirements).</t>
+          <t>A document is open with a requirement whose description contains a known XSS payload (e.g., &lt;script&gt;alert('XSS');&lt;/script&gt;, &lt;img src=x onerror=alert('XSS')&gt;).</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>1. Select a requirement. 2. Use the 'Mark as Deleted' action. 3. Verify the requirement is visually marked as deleted (e.g., greyed out, strike-through). 4. With the same requirement selected, use the 'Undelete' action. 5. Verify the requirement is restored to its original state. 6. Mark the requirement as deleted again. 7. With the deleted requirement selected, use the 'Permanently Remove' action. 8. Verify the requirement is no longer visible. 9. Select a section containing requirements. 10. Use the 'Mark as Deleted' action on the section. 11. Verify the section and its contents are visually marked as deleted. 12. Use 'Permanently Remove' on the deleted section. 13. Verify the section and its contents are removed.</t>
+          <t>1. Ensure the requirement with the XSS payload is visible in the document.
+2. Click 'File' -&gt; 'Export' -&gt; 'HTML'.
+3. Save the HTML file and open it in a web browser.</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>The requirement is marked as deleted. The requirement is successfully undeleted and reverts to its original state. The deleted requirement is permanently removed from the document and is no longer visible. The selected section and all its contained requirements are marked as deleted. The deleted section and its contents are permanently removed from the document.</t>
+          <t>The exported HTML file displays the requirement's content, but the XSS payload is sanitized (e.g., script tags removed, characters escaped, event handlers stripped). The malicious script is NOT executed in the browser. The exported HTML content is safe to view.</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -840,27 +870,31 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>TC013</t>
+          <t>TC_VIEW_001</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Verify editing section heading and requirement text description with pasted HTML content, including large and malformed content.</t>
+          <t>Verify the document view correctly displays the Table of Contents and Requirements Table, including all configured attributes.</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>An opened document with at least one section and one requirement.</t>
+          <t>A document with multiple sections, requirements (including custom attributes, links, and discussions), and varying levels of hierarchy is open.</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>1. Select a section. 2. Use the 'Edit Heading' action and change the text to a new string. 3. Select a requirement. 4. Open its description for editing. 5. Copy some rich HTML content (e.g., a complex table with formatted text, embedded images if supported) from MS Word. 6. Paste the HTML content into the requirement's description field. 7. Save changes. 8. (Edge) Paste a very large amount of plain text (e.g., 100,000+ characters) into a description. 9. (Negative) Paste malformed HTML (e.g., unclosed tags, invalid attributes) into a description.</t>
+          <t>1. Open the document.
+2. Observe the left-hand Table of Contents (TOC) pane.
+3. Observe the main Requirements Table area.
+4. Verify displayed columns (ID, Description, Discussion, Links, all configured custom attributes).
+5. Interact with the view (scroll, resize panes).</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>The section heading is successfully updated and displayed. The pasted HTML content is correctly rendered in the requirement's description, retaining its formatting (e.g., table structure, bold, italics, images). Very large text is accepted and displayed, potentially with scrollbars. Malformed HTML is either sanitized and displayed correctly, or an error/warning is shown, but the application does not crash and the document remains valid.</t>
+          <t>The Table of Contents displays correctly with hierarchical section headings, reflecting the document structure. The Requirements Table displays with 'ID', 'Description', 'Discussion', 'Links', and all configured custom attribute columns. All content (text, rich text, attribute values) is legible, correctly formatted, and accurately reflects the document data. Scrolling and resizing panes are smooth and responsive, even for documents with many items.</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -872,283 +906,302 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>TC014</t>
+          <t>TC_VIEW_002</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Verify defining and setting values for different custom attribute types (Enum, XHTML, Integer, String, Date/Time), including boundary and negative cases.</t>
+          <t>Verify application prevents hiding the 'ID' column in the requirements table.</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>An opened document. Access to custom attribute definition settings.</t>
+          <t>A document with requirements is open and displayed.
+The 'ID' column is visible.</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>1. Define a custom attribute of type 'Enum' named 'Priority' with values 'High', 'Medium', 'Low', 'Critical'. 2. Define a custom attribute of type 'XHTML' named 'RichNotes'. 3. Define a custom attribute of type 'Integer' named 'Effort'. 4. Define a custom attribute of type 'String' named 'Status'. 5. Define a custom attribute of type 'Date/Time' named 'DueDate'. 6. Select a requirement. 7. Set 'Priority' to 'High'. Then attempt to set it to 'Critical' (multi-value enum if supported, or single choice). 8. Enter rich text into 'RichNotes'. 9. Enter '5' into 'Effort', then try '0', then '-1' (negative), then max/min integer value, then 'abc' (non-integer). 10. Enter a very long string (e.g., 500+ characters) into 'Status'. 11. Set 'DueDate' to a valid date, then an invalid date (e.g., Feb 30). 12. (Negative) Attempt to define a custom attribute with an existing ID (as per TC024).</t>
+          <t>1. Attempt to hide the 'ID' column using all available UI methods (e.g., right-click column header and look for 'Hide' option, drag it off, check view settings).</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Custom attributes 'Priority', 'RichNotes', 'Effort', 'Status', 'DueDate' are successfully defined. The requirement's 'Priority' attribute correctly stores the selected enum value(s). 'RichNotes' displays the rich text formatting. 'Effort' stores valid integer values correctly; invalid input like 'abc' results in an error/rejection, and boundary values (max/min int) are handled. 'Status' accepts and displays very long strings. 'DueDate' accepts valid dates and rejects invalid ones. Defining custom attributes with non-unique IDs is prevented.</t>
+          <t>The application prevents the 'ID' column from being hidden. The 'Hide' option for the ID column is disabled, grayed out, or the action has no effect. The 'ID' column remains visible and fixed in its position.</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>High</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>TC015</t>
+          <t>TC_VIEW_003</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Verify attaching multiple documents, saving them, and removing them from a requirement, including security and error handling.</t>
+          <t>Verify application prevents sorting 'Discussion' or 'Links' columns.</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>An opened document with a selected requirement. Multiple local files of various types (e.g., PDF, Word, Excel, image, an empty file, a very large file, a file with special characters in name) are available. A locked file is also prepared. A suspicious file type (e.g., '.exe', '.bat') is also available.</t>
+          <t>A document with requirements is open and displayed, and these columns are visible.</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>1. Select a requirement. 2. Use the 'Attach File' action. 3. Select multiple valid files (e.g., 'report.pdf', 'spec.docx', 'diagram.png', 'empty.txt', 'long_name_file_!@#$%^&amp;.jpg') and attach them. 4. Verify all files appear as attachments. 5. Select an attachment and use 'Save Attachment As' to save it locally. 6. Verify the saved attachment matches the original. 7. Select an attachment and use 'Remove Attachment' action. 8. Confirm removal. 9. (Negative) Attempt to attach a non-existent file. 10. (Negative) Attempt to attach a locked file. 11. (Negative) Attempt to attach a very large file (e.g., 1GB) or a file exceeding a defined attachment size limit. 12. (Security) Attempt to attach a suspicious file type (e.g., 'virus.exe'). 13. During an attachment operation, click 'Cancel'.</t>
+          <t>1. Attempt to sort the 'Discussion' column (e.g., click on the column header).
+2. Attempt to sort the 'Links' column (e.g., click on the column header).</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>All selected valid files are successfully attached to the requirement and listed. The saved attachment file matches the original content. The selected attachment is permanently removed from the requirement. An error message is displayed for non-existent files. An error message is displayed for locked files. An error/warning is displayed or the operation is prevented for files exceeding size limits. Suspicious file types might be prevented from attaching or a security warning displayed, but the application does not crash. The attachment operation is aborted when 'Cancel' is clicked.</t>
+          <t>The application prevents sorting the 'Discussion' and 'Links' columns. Clicking the headers of these columns has no effect on the sorting of requirements. The UI indicates that these columns are not sortable (e.g., no sort icon appears).</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>High</t>
+          <t>Medium</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>TC016</t>
+          <t>TC_EDIT_STRUCT_001</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Verify commenting a requirement and expanding/collapsing comments in the discussion pane, including security aspects.</t>
+          <t>Verify user can successfully create a new requirement within a specified document section.</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>An opened document with a selected requirement.</t>
+          <t>A document with at least one section is open.</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>1. Select a requirement. 2. Use the 'Comment' action and add a comment ('This is comment 1.'). 3. Add another comment ('This is comment 2.'). 4. (Edge) Add a very long comment (e.g., 1000+ characters). 5. (Security) Add a comment containing malicious script (e.g., &lt;script&gt;alert('XSS Comment!');&lt;/script&gt;). 6. Ensure the Discussion pane is visible. 7. Verify all comments are displayed, ordered by date/time, with author and timestamp. 8. Click to expand a collapsed comment. 9. Click to collapse an expanded comment. 10. Use 'Expand All' then 'Collapse All' actions. 11. (Negative) Attempt to add an empty comment.</t>
+          <t>1. Select an existing document section in the TOC or Requirements Table where the new requirement should be added.
+2. Click 'Add Requirement' or equivalent action (e.g., context menu, toolbar button).
+3. Enter a valid description for the new requirement.
+4. Save or allow auto-save.</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>The comments are successfully added and displayed in the Discussion pane, ordered correctly by date/time, with accurate author and timestamp information. Very long comments are displayed correctly, possibly with truncation or scrollbars. Malicious script in comments is sanitized and displayed as plain text or escaped HTML, NOT executed. Individual comments expand and collapse as expected. 'Expand All' and 'Collapse All' actions correctly modify the display state of all comments. Attempting to add an empty comment is prevented or results in a warning.</t>
+          <t>A new requirement is created and correctly placed as a child of the selected document section. It is assigned a unique, immutable ID according to the document's ID schema. The requirement is immediately visible in the requirements table under its parent section. No errors are shown.</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>High</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>TC017</t>
+          <t>TC_EDIT_STRUCT_001_NEG_001</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Verify defining a new link type, creating a directed traceability link, changing its type, and removing it, including negative and edge cases.</t>
+          <t>Verify application handles creating a requirement with an empty description (if description is mandatory).</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>An opened document with at least two requirements (Req A, Req B, Req C). Access to link type definition settings. A deleted requirement exists.</t>
+          <t>A document is open. Description is a mandatory field for requirements.</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>1. Define a new link type 'Refines' with role 'refines'. 2. Define another link type 'Verifies' with role 'verifies'. 3. Select Req A and Req B. 4. Create a directed traceability link of type 'Refines' from Req A to Req B. 5. Verify the link is displayed in the 'Links' pane for both requirements, showing directionality. 6. Select the created link. 7. Change its link type to 'Verifies'. 8. Verify the link type is updated. 9. Select Req C. 10. (Negative) Attempt to create a link from Req C to a non-existent requirement ID. 11. (Negative) Attempt to create a link from Req C to a deleted requirement. 12. (Negative) Attempt to create a circular link (e.g., A -&gt; B, then B -&gt; A with a different link type). 13. (Edge) Create a requirement with a very large number of incoming and outgoing links (e.g., 100+). 14. Select the 'Verifies' link and use 'Remove Traceability Link'.</t>
+          <t>1. Select a section.
+2. Initiate 'Add Requirement'.
+3. Attempt to save the new requirement with an empty description.</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>The 'Refines' and 'Verifies' link types are successfully defined. A directed link from Req A to Req B is created and displayed. The link type is successfully changed to 'Verifies'. Link creation to a non-existent or deleted requirement is prevented with an error. Circular links are allowed and displayed correctly (or prevented if design choice). A requirement with many links displays them efficiently without performance degradation. The traceability link is permanently removed from the document.</t>
+          <t>The application displays an error message (e.g., 'Description cannot be empty', 'Please enter a description') and prevents the creation of the requirement until a valid description is provided. The application remains stable.</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>High</t>
+          <t>Medium</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>TC018</t>
+          <t>TC_EDIT_STRUCT_001_BOUNDARY_001</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Verify document changes are automatically persisted (for crash recovery) and restored upon unexpected application termination.</t>
+          <t>Verify application handles creating a requirement with an extremely long description.</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Application is running. No document is currently open (or open a new one).</t>
+          <t>A document is open.</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>1. Create a new document. 2. Create a new section and a new requirement. 3. Add some text to the requirement description. 4. Do NOT explicitly save. 5. Force-quit the application (e.g., Task Manager -&gt; End Task, or kill process) without going through normal shutdown. 6. Restart the application. 7. Open the previously created document.</t>
+          <t>1. Select a section.
+2. Initiate 'Add Requirement'.
+3. Paste or type a very long string (e.g., 65,535 characters or more, if system supports it) into the description field.
+4. Save the requirement.</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>The application crashes gracefully (no data corruption). Upon restart and opening the document, the newly created section, requirement, and its description text are all present and correctly restored, indicating successful automatic persistence/crash recovery. No 'Save Changes' prompt should appear during the force-quit if auto-persistence is intended to handle crashes.</t>
+          <t>The requirement is successfully created with the extremely long description. The application should handle the text without truncation, corruption, or performance issues when displaying/editing. If there is a practical limit, the application should gracefully truncate or provide a warning, not crash.</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>High</t>
+          <t>Medium</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>TC019</t>
+          <t>TC_EDIT_STRUCT_002</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Verify filtering requirements using a complex DNF condition and searching with multiple keywords, including edge cases and invalid syntax.</t>
+          <t>Verify user can successfully move an existing document section within the document hierarchy.</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>An opened document with diverse requirements, sections, and custom attributes (e.g., 'Priority' enum, 'Status' string, 'Description' text) that allow for a range of filter matches and search keywords.</t>
+          <t>A document with at least two sections is open, where one can be moved under another.</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>1. Enter a complex DNF filter condition (e.g., '(Priority = High AND Status = New) OR (Description CONTAINS 'critical issue' AND Effort &gt; 5)'). 2. Verify only requirements matching the condition are displayed. 3. Clear the filter. 4. (Edge) Enter a filter condition that matches all requirements. 5. (Edge) Enter a filter condition that matches no requirements. 6. (Negative) Enter an invalid filter syntax (e.g., missing parenthesis). 7. Clear the filter. 8. Open the search function. 9. Enter multiple keywords (e.g., 'user interface design') into the search box. 10. Click 'Search', then 'Next', then 'Previous' to navigate matches. 11. (Edge) Search for a very long keyword string. 12. (Edge) Search for keywords using special characters (e.g., 'C++' or 'Req#123').</t>
+          <t>1. Select a document section (e.g., 'Section 2') in the TOC.
+2. Use the 'Move' function (e.g., drag-and-drop, context menu 'Move' option with target selection) to move 'Section 2' under 'Section 1'.
+3. Observe the TOC and Requirements Table.
+4. Verify the IDs of requirements and sections, and any links, are still valid.</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Only requirements matching the complex DNF condition are displayed correctly. Filtering to all/no requirements works as expected. Invalid filter syntax results in an error message. The search function finds and highlights all occurrences of the keywords across relevant fields. 'Next' and 'Previous' correctly navigate between matched items. Long keyword strings are searchable. Special characters are correctly interpreted in searches.</t>
+          <t>The selected document section, along with all its child requirements and sub-sections, is successfully moved to the new location. The hierarchy in the TOC and requirements table updates accordingly. All associated IDs remain consistent, and any existing traceability links remain valid and correctly point to the moved items. The application remains stable and responsive.</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>High</t>
+          <t>Medium</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>TC020</t>
+          <t>TC_EDIT_STRUCT_002_NEG_001</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Verify printing the displayed requirements table and creating a PDF, including handling of large documents and printer status.</t>
+          <t>Verify application prevents moving a section to create a circular reference (e.g., moving a parent into its own child).</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>An opened document with requirements displayed. A printer is configured (or a virtual PDF printer). A document with complex tables/images/many pages is available.</t>
+          <t>A document with a nested structure (e.g., Section A -&gt; Section B) is open.</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>1. Apply a filter to display a subset of requirements. 2. Navigate to 'File' menu. 3. Select 'Print'. 4. Review the print preview (if available) and confirm print. 5. (Negative) Simulate an offline printer and attempt to print. 6. Navigate to 'File' menu. 7. Select 'Create PDF'. 8. Choose a destination path and file name (e.g., 'Report.pdf'). 9. Click 'Save'. 10. (Edge) Print/PDF a document with very complex tables, images, or a large number of pages (e.g., 50+ pages). 11. During a print or PDF creation operation, click 'Cancel'.</t>
+          <t>1. Select 'Section A' (parent).
+2. Attempt to move 'Section A' to become a child of 'Section B' (its current child) using the UI.</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>The filtered requirements table is sent to the printer and prints correctly, matching the displayed view. A PDF file is successfully generated and saved, containing the displayed requirements table with its current formatting and filtering. An error message is displayed when attempting to print to an offline printer. Complex and multi-page documents print/PDF correctly with proper pagination and layout. The print/PDF operation is aborted when 'Cancel' is clicked.</t>
+          <t>The application prevents this action, either by disabling the target location, displaying an error message (e.g., 'Cannot move a parent into its own child', 'Invalid move operation'), or by reverting the action. The document hierarchy remains consistent and valid. The application remains stable.</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>High</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>TC021</t>
+          <t>TC_EDIT_STRUCT_002_EDGE_001</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Verify application runs completely offline and clears session-specific persisted data on document close.</t>
+          <t>Verify user can successfully move a section to become a root-level section.</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Application is closed. No active internet connection. An existing document is available.</t>
+          <t>A document with a nested section (e.g., Section 1 -&gt; Section 1.1) is open.</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>1. Disconnect from the internet. 2. Start the application. 3. Open an existing document. 4. Perform some edits (e.g., add a requirement, change a custom attribute). 5. Close the document (without saving changes if prompted). 6. Re-open the same document. 7. Connect to the internet. 8. Observe if any deferred online operations are initiated.</t>
+          <t>1. Select 'Section 1.1'.
+2. Use the 'Move' function to move 'Section 1.1' to the root level of the document, making it a peer of 'Section 1'.
+3. Observe the TOC and Requirements Table.</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>The application starts and operates normally without requiring any server connection or displaying connectivity errors. All local edits (made prior to closing) are persisted to the document file (due to auto-save or user prompt handling as per TC025). Any session-specific temporary persisted data (e.g., undo history, temporary caches not part of the document file) is cleared. Upon re-opening, the document reflects the state when last closed/saved. No deferred online operations occur upon internet reconnection, confirming offline capability.</t>
+          <t>The selected section ('Section 1.1') and all its children are successfully moved to the root level. The hierarchy in the TOC and table updates accordingly. The application remains stable.</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Low</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>TC022</t>
+          <t>TC_EDIT_ATTR_001</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Attempt to open a non-existent, corrupted, or locked file, and save to a read-only or non-existent location.</t>
+          <t>Verify user can successfully edit the rich text description of a selected requirement.</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Application is running. A non-existent file path, a corrupted document file, and a valid document file currently locked by another application are prepared. A read-only directory and a non-existent directory exist.</t>
+          <t>A document with requirements is open. A requirement with an existing description is selected.</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>1. Navigate to 'File' menu. 2. Select 'Open Document'. 3. Enter a path to a non-existent file and click 'Open'. 4. Select 'Open Document' again. 5. Choose the corrupted document file and click 'Open'. 6. Select 'Open Document' again. 7. Choose the locked document file and click 'Open'. 8. Create a new document. 9. Navigate to 'File' menu. 10. Select 'Save As'. 11. Choose the read-only directory and attempt to save. 12. Choose a non-existent directory and attempt to save.</t>
+          <t>1. Select a requirement.
+2. Edit its description in the requirements table or detailed information pane (e.g., change text, apply bold, italics, underline formatting, add a bulleted list, add a hyperlink).
+3. Save or allow auto-save.
+4. Re-open the document or navigate away and back to the requirement.</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>An appropriate error message is displayed for the non-existent file (e.g., 'File not found'). An appropriate error message is displayed for the corrupted file (e.g., 'Invalid file format', 'Document corrupted'). An error message is displayed indicating the file is locked or in use by another process. An error message is displayed preventing save to the read-only location (e.g., 'Permission denied'). An error message is displayed when attempting to save to a non-existent directory.</t>
+          <t>The requirement's text description is successfully updated, including all applied rich text formatting. The changes are displayed correctly and persistently in the UI (table, detail pane). The hyperlink is functional. No errors are displayed, and the application remains stable.</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -1160,27 +1213,30 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>TC023</t>
+          <t>TC_EDIT_ATTR_002</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Attempt to hide the ID column and sort the Links or Discussion columns, which are typically non-modifiable.</t>
+          <t>Verify application handles pasting malformed/invalid HTML content (XSS vulnerability check) into a requirement description.</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>An opened document is displayed with standard columns visible.</t>
+          <t>A document with requirements is open. A requirement is selected for editing its description. Malformed HTML strings or known XSS payloads (e.g., &lt;script&gt;alert('xss');&lt;/script&gt;, &lt;p&gt;&lt;b&gt;unclosed tag, &lt;img src='x' onerror='alert(1)'&gt;) are available in clipboard.</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>1. Navigate to column visibility settings (e.g., right-click column header -&gt; 'Columns' or 'View' menu). 2. Attempt to uncheck/hide the 'ID' column. 3. Click on the 'Links' column header to attempt sorting. 4. Click on the 'Discussion' column header to attempt sorting.</t>
+          <t>1. Select a requirement.
+2. Open its rich text description editor.
+3. Attempt to paste malformed/invalid HTML or XSS payloads into the editor.
+4. Save or observe the editor's behavior and the displayed content.</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>The option to hide the 'ID' column is disabled, greyed out, or uncheckable, preventing it from being hidden. Clicking the 'Links' column header has no effect on sorting; requirements do not reorder. Clicking the 'Discussion' column header has no effect on sorting; requirements do not reorder, indicating sorting is not supported for these columns.</t>
+          <t>The application either sanitizes the malformed HTML, removing potentially harmful or breaking elements (e.g., scripts, event handlers), or displays an error/warning and prevents pasting. The application remains stable, the document content is not corrupted, and no malicious scripts are executed.</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -1192,27 +1248,33 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>TC024</t>
+          <t>TC_CUSTOM_ATTR_001</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Attempt to permanently remove a non-deleted requirement and define a custom attribute with a non-unique ID.</t>
+          <t>Verify user can successfully define a new custom enumeration attribute with multiple values.</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>An opened document with an active (not deleted) requirement. Access to custom attribute definition settings. A custom attribute named 'Status' (type String) already exists.</t>
+          <t>Application is launched and a document is open. User has permissions to manage custom attributes.</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>1. Select an active (not deleted) requirement. 2. Attempt to use the 'Permanently Remove' action (e.g., via menu or context click). 3. Open custom attribute definition settings. 4. Define a new custom attribute (e.g., 'Status', type String, if not already existing from preconditions). 5. Attempt to define another custom attribute with the exact same ID (e.g., 'Status', type Enum). 6. Attempt to define a new custom attribute without providing an ID.</t>
+          <t>1. Go to 'Custom Attributes Management' settings.
+2. Click 'Add New Attribute'.
+3. Set a unique and valid name for the attribute (e.g., 'Status').
+4. Set the type to 'Enumeration'.
+5. Add multiple distinct values to the enumeration list (e.g., 'Open', 'In Progress', 'Done').
+6. Save the custom attribute definition.
+7. Verify its availability for requirements.</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>The 'Permanently Remove' action for the active requirement is disabled, greyed out, or displays an error indicating the requirement must be marked as deleted first. The application prevents defining a custom attribute with a non-unique ID, displaying an error message (e.g., 'Attribute ID already exists'). The application prevents defining a custom attribute without an ID, displaying a 'missing ID' error.</t>
+          <t>A new custom attribute of type 'Enumeration' is successfully defined with the specified name and values. It is assigned a unique, immutable ID. The attribute becomes available for assignment to requirements in the document and appears in the list of managed attributes. No errors are displayed.</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -1224,315 +1286,351 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>TC025</t>
+          <t>TC_CUSTOM_ATTR_001_NEG_001</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Attempt to close a document with unsaved changes and choose not to save, verifying data discard.</t>
+          <t>Verify application prevents defining a custom attribute with an empty or duplicate name.</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>An opened document where changes have been made but not yet explicitly saved by the user (assuming auto-persistence from TC018 is for recovery, not replacing explicit save prompts).</t>
+          <t>Application is launched and a document is open.</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>1. Open an existing document. 2. Make a significant change (e.g., add a requirement, delete a section, edit description). 3. Immediately attempt to close the document (e.g., File -&gt; Close, or application close button). 4. When prompted to save changes, choose 'Don't Save' (or equivalent option). 5. Re-open the same document.</t>
+          <t>1. Go to 'Custom Attributes Management'.
+2. Attempt to add a new attribute with an empty name.
+3. Attempt to add a new attribute with a name that already exists for another custom attribute.</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>A prompt appears asking if changes should be saved. Upon selecting 'Don't Save', the document closes without saving the changes. When re-opening the same document, the changes made in step 2 are *not* present, confirming they were successfully discarded. The document reverts to its state prior to the changes made in step 2.</t>
+          <t>In both cases, the application displays an error message (e.g., 'Attribute name cannot be empty', 'An attribute with this name already exists') and prevents the creation of the attribute. The application remains stable.</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>High</t>
+          <t>Medium</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>TC026</t>
+          <t>TC_CUSTOM_ATTR_001_NEG_002</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Verify error handling when attempting to save a document to a full or critically low storage drive.</t>
+          <t>Verify application prevents defining an enumeration attribute with duplicate or empty enumeration values.</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Application is running with an opened document. The designated storage drive for saving is full or has critically low space (e.g., less than 1KB free).</t>
+          <t>Application is launched and a document is open.</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>1. Make some changes to the opened document (ensure the document size + changes would exceed remaining disk space). 2. Navigate to 'File' menu. 3. Select 'Save'. 4. (Negative) Repeat steps 1-2, but with a network drive that unexpectedly becomes unavailable or loses connection during the save operation.</t>
+          <t>1. Go to 'Custom Attributes Management'.
+2. Add a new enumeration attribute.
+3. Attempt to add two identical enumeration values (e.g., 'Value A', 'Value A').
+4. Attempt to add an empty string as an enumeration value.</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>An error message is displayed indicating the save operation failed due to insufficient disk space (e.g., 'Disk full', 'Cannot write to file', 'Out of disk space'). The document should remain in its unsaved state. For network drive issues, an error message indicating network problems or loss of connection should be displayed.</t>
+          <t>The application displays an error or warning message (e.g., 'Duplicate enumeration value', 'Value cannot be empty') and prevents the addition of invalid values. The attribute definition remains valid or is prevented from saving until corrected. The application remains stable.</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>High</t>
+          <t>Medium</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>TC027</t>
+          <t>TC_CUSTOM_ATTR_001_BOUNDARY_001</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Verify application performance for opening a large document (10,000 objects, 100MB) within defined time limits.</t>
+          <t>Verify application handles defining a custom attribute with a very long name or very long enumeration values.</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Application is closed. A large document file (approx. 10,000 objects and 100MB total size) is available locally.</t>
+          <t>Application is launched and a document is open.</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>1. Start a timer. 2. Launch the application. 3. Open the large document. 4. Stop the timer when the document content is fully displayed, interactive, and all panes (TOC, details) are populated and responsive.</t>
+          <t>1. Go to 'Custom Attributes Management'.
+2. Attempt to define a new attribute with a name exceeding typical character limits (e.g., 255+ characters).
+3. For an enumeration type, add values that are also very long strings.
+4. Save the attribute.</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>The large document is fully displayed and interactive within 10 seconds. No 'Application Not Responding' messages or significant UI freezes occur during load. All UI elements (scrolling, clicking requirements, opening panes) respond promptly after load.</t>
+          <t>The application should either successfully save the attribute with the long name/values (if supported by the backend) or truncate the input and inform the user, or display a clear error message about character limits. The application remains stable and the UI renders the long names/values without corruption.</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>High</t>
+          <t>Low</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>TC028</t>
+          <t>TC_CUSTOM_ATTR_002</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Verify behavior with a completely empty document and rejection when exceeding document size or object count limits.</t>
+          <t>Verify removing a custom attribute also unsets its values in all requirements and removes it from UI.</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Application is running. A new empty document is opened. Document size limit is 100MB, object limit is 10,000.</t>
+          <t>A custom attribute is defined and assigned values to at least two different requirements. This attribute is visible in the requirements table.</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>1. Create a new empty document. 2. Verify UI elements are appropriate for an empty document (e.g., 'No requirements yet' message, disabled actions like 'Copy', 'Move'). 3. Attempt to continuously add requirements and large attachments (via script or rapid manual creation) to reach/exceed the 100MB total size limit. 4. Attempt to continuously add requirements (minimal content) to reach/exceed the 10,000 object limit.</t>
+          <t>1. Navigate to 'Custom Attributes Management' settings.
+2. Select the custom attribute that has assigned values.
+3. Click 'Remove Attribute' and confirm the action in any dialog.
+4. Observe the requirements where the attribute was previously assigned (e.g., in the requirements table, detail pane).
+5. Verify the attribute is no longer listed in custom attribute management.</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>The application correctly displays an empty state with relevant actions disabled. When attempting to exceed the document size limit (100MB), the application should prevent further creation of large attachments/content or display a warning/error message (e.g., 'Document size limit reached'). When attempting to exceed the object limit (10,000), the application should prevent further requirement/section creation or display a warning/error message (e.g., 'Maximum object count reached'). The application should remain stable.</t>
+          <t>The custom attribute is successfully removed from the definitions. In all requirements where this attribute had a value, its value is unset/cleared, and the attribute column/field no longer appears in the requirements table or detailed pane. The attribute is completely gone from the system's configuration. No errors are displayed.</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>High</t>
+          <t>Medium</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>TC029</t>
+          <t>TC_ATTACH_001</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Verify inputting very long strings, special characters, and emoji into text fields and their display, including boundary checks.</t>
+          <t>Verify user can successfully attach an image file to a selected requirement.</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>An opened document with a requirement, section, and custom string/XHTML attributes.</t>
+          <t>A document with requirements is open. A requirement is selected.
+A valid image file (e.g., .png, .jpg, .gif) of a reasonable size is available locally.</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>1. Edit a section heading with a very long string (e.g., 250+ characters, up to system limit). 2. Edit a requirement description with a very long string (e.g., tens of thousands of characters), including various special characters (e.g., !@#$%^&amp;*()_+-=[]{};:'",.&lt;&gt;/?|), common Unicode characters, and emojis. 3. Create a custom string attribute and enter a very long string with special characters/emoji. 4. Enter a string consisting only of whitespace characters (spaces, tabs, newlines) into a description. 5. Save and view the document.</t>
+          <t>1. Select a requirement.
+2. Access the 'Attachments' management feature for the selected requirement.
+3. Click 'Add Attachment' and select the image file.
+4. Confirm attachment (if prompted).
+5. Verify the attachment is listed and can be previewed/opened.</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>The application accepts and displays very long strings without truncation or errors, respecting UI boundaries (e.g., wrapping, scrollbars). All special characters, common Unicode characters, and emojis are correctly rendered and displayed in headings, descriptions, and custom attribute fields without corruption, unexpected behavior, or encoding issues. Strings with only whitespace are also correctly displayed.</t>
+          <t>The image file is successfully attached to the selected requirement. The attachment appears in the attachments list for that requirement, showing its name and size. The attachment's content can be previewed directly within the application (if supported) or opened externally via a double-click/context menu, displaying the correct image. No errors are shown.</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>High</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>TC030</t>
+          <t>TC_ATTACH_001_BOUNDARY_001</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Verify XSS prevention when displaying malicious script input in requirement descriptions or custom XHTML attributes.</t>
+          <t>Verify application handles attaching a very large image file.</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>An opened document. A requirement with editable description. A custom XHTML attribute defined.</t>
+          <t>A document with requirements is open. A requirement is selected.
+A very large image file (e.g., 50MB+, depending on system limits) is available locally.</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>1. Edit a requirement's description. 2. Paste malicious script (e.g., &lt;script&gt;alert('XSS Attack!');&lt;/script&gt;&lt;img src='x' onerror='alert("Image XSS!")'&gt;) into the description. 3. Save the description. 4. View the requirement description. 5. Edit a custom XHTML attribute for a requirement. 6. Paste the same malicious script into the XHTML attribute. 7. Save and view the custom attribute. 8. Export the document to HTML and open the HTML file in a browser.</t>
+          <t>1. Select a requirement.
+2. Access the 'Attachments' management feature.
+3. Click 'Add Attachment' and select the large image file.
+4. Confirm attachment.</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>The malicious script is sanitized and displayed as plain text or escaped HTML entities in both the requirement description and the custom XHTML attribute. The script is NOT executed, and no alert box or other malicious behavior occurs, confirming XSS prevention. When exported to HTML, the malicious script is also sanitized or escaped in the generated HTML, preventing execution in the browser.</t>
+          <t>The application successfully attaches the large image file (within defined system limits). The attachment process completes within an acceptable time frame. The application remains responsive, and the attached file can be downloaded/opened without corruption. If there is a file size limit, an appropriate error message should be displayed.</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>High</t>
+          <t>Medium</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>TC031</t>
+          <t>TC_ATTACH_002</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Verify basic Undo/Redo functionality for common editing operations.</t>
+          <t>Verify application prevents attaching files of explicitly unsupported formats.</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>An opened document with at least one requirement.</t>
+          <t>A document with requirements is open. A requirement is selected.
+An explicitly unsupported file type (e.g., .psd, .ai, .raw, or other document-specific forbidden types) is available locally.</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>1. Create a new requirement. 2. Use 'Undo' action. 3. Verify the requirement is removed. 4. Use 'Redo' action. 5. Verify the requirement is re-added. 6. Edit a requirement's description. 7. Use 'Undo'. 8. Verify the description reverts. 9. Use 'Redo'. 10. Verify the description returns to edited state. 11. Delete a requirement. 12. Use 'Undo'. 13. Verify the requirement is restored. 14. Use 'Redo'. 15. Verify the requirement is deleted again.</t>
+          <t>1. Select a requirement.
+2. Access the 'Attachments' management feature.
+3. Attempt to attach the unsupported file type.</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>The 'Undo' and 'Redo' actions successfully reverse and re-apply changes for creation, editing, and deletion of requirements. The UI updates correctly at each step.</t>
+          <t>The application displays a clear error message indicating that the file type is unsupported/not allowed (e.g., 'Unsupported file format', 'Invalid file type') and prevents the attachment. The application remains stable.</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>High</t>
+          <t>Medium</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>TC032</t>
+          <t>TC_ATTACH_002_SEC_001</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Verify Cut/Copy/Paste operations for requirements and sections via system clipboard.</t>
+          <t>Verify application prevents attaching known malicious executable files or scripts.</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>An opened document with multiple requirements and sections.</t>
+          <t>A document with requirements is open. A requirement is selected.
+Known malicious file types (e.g., .exe, .bat, .vbs, .js, .dll, .scr) are available locally.</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>1. Select a requirement. 2. Use 'Copy' action. 3. Select a different section. 4. Use 'Paste' action. 5. Verify a new requirement is created. 6. Select a requirement. 7. Use 'Cut' action. 8. Select a different section. 9. Use 'Paste' action. 10. Verify the requirement is moved and its original location is empty. 11. Repeat steps 1-10 for a document section (copy/cut a section, paste into another, paste at top level). 12. (Negative) Attempt to paste non-requirement/section content from clipboard.</t>
+          <t>1. Select a requirement.
+2. Access the 'Attachments' management feature.
+3. Attempt to attach each of the malicious file types.</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Copied requirements/sections are successfully pasted, creating new unique IDs for copied items. Cut requirements/sections are successfully moved to the new location, with their original position becoming empty. Pasted sections retain their hierarchical structure and contained requirements. Attempting to paste non-document content either does nothing or provides an appropriate message.</t>
+          <t>The application explicitly prevents the attachment of these potentially dangerous file types, displaying an error message (e.g., 'Forbidden file type', 'Security risk detected'). No attempt should be made to execute or process the file content, and the application remains secure and stable.</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>High</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>TC033</t>
+          <t>TC_ATTACH_002_EDGE_001</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Verify Drag and Drop functionality for reordering requirements and sections within the document.</t>
+          <t>Verify application handles attaching files with no extension or deceptive extensions.</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>An opened document with multiple requirements and sections.</t>
+          <t>A document with requirements is open. A requirement is selected.
+Files with no extension, or with a double extension (e.g., document.txt.exe), or with a common file type but containing malicious content, are available.</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>1. Select a requirement. 2. Drag it to a new position within the same section. 3. Verify the requirement's position is updated. 4. Drag the same requirement to a different section, making it a child of that section. 5. Verify the requirement is moved and its parent section is updated. 6. Select a document section. 7. Drag it to a new position (e.g., reorder with sibling sections). 8. Verify the section is moved and its numbering updated. 9. Drag the same section to become a sub-section of another section. 10. Verify the section and its contents are moved and re-parented.</t>
+          <t>1. Select a requirement.
+2. Access the 'Attachments' management feature.
+3. Attempt to attach a file with no extension.
+4. Attempt to attach a file with a double extension (e.g., image.jpg.exe).
+5. Attempt to attach a file disguised as a safe type but internally containing dangerous code (if system checks content).</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>Requirements and sections can be successfully reordered and re-parented via drag and drop. The UI provides clear visual feedback during drag operations. All changes (position, parent, numbering) are correctly reflected in the document structure.</t>
+          <t>The application should handle these cases securely. Files with no extension might be allowed if content inspection deems them safe, or blocked by default. Files with deceptive extensions should be blocked or warned against. The application should prioritize security over convenience, preventing potential attacks. An appropriate warning or error message is displayed. The application remains stable.</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>High</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>TC034</t>
+          <t>TC_COMMENTS_001</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Verify editing requirement content (description, discussion, links) and section headings.</t>
+          <t>Verify user can add a comment to the selected requirement, with author, date, and time recorded.</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>An opened document with requirements and sections.</t>
+          <t>A document with requirements is open. A requirement is selected.
+The 'Discussion' pane is visible.</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>1. Select a section. 2. Double-click or use 'Edit' action to modify its heading text. 3. Save changes. 4. Select a requirement. 5. Double-click or use 'Edit' action to modify its description text. 6. Save changes. 7. Add a new comment to a requirement. 8. (If editable) Attempt to edit an existing comment. 9. (If editable) Attempt to edit a traceability link's properties (e.g., description, type).</t>
+          <t>1. Select a requirement.
+2. Navigate to the 'Discussion' pane.
+3. Enter valid text (e.g., 'This requirement needs clarification.') into the comment input field.
+4. Click 'Add Comment' or equivalent action.</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Section headings are successfully editable and changes persist. Requirement descriptions are successfully editable, supporting rich text as per TC013, and changes persist. New comments are added correctly. If comments/links are editable, changes should persist correctly.</t>
+          <t>The new comment is successfully added to the selected requirement. The comment is displayed in the discussion pane, showing the full comment text, the current user's name (author), the exact date, and time of creation. The comments are ordered chronologically. No errors are displayed.</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -1544,27 +1642,31 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>TC035</t>
+          <t>TC_COMMENTS_001_NEG_001</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Verify application settings and preferences (e.g., language, default paths, UI theme).</t>
+          <t>Verify application prevents adding an empty comment.</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Application is running. Access to 'Settings' or 'Preferences' menu.</t>
+          <t>A document with requirements is open. A requirement is selected.
+The 'Discussion' pane is visible.</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>1. Navigate to 'Settings' or 'Preferences'. 2. Change a UI theme (e.g., Light to Dark). 3. Apply changes and verify the UI theme updates. 4. Change the default save path for new documents. 5. Create a new document and attempt to save it (verify default path is new one). 6. Change the application language (if supported). 7. Restart the application and verify the language. 8. (Negative) Enter an invalid value for a numeric setting (e.g., negative value for 'max attachments').</t>
+          <t>1. Select a requirement.
+2. Navigate to the 'Discussion' pane.
+3. Leave the comment input field empty.
+4. Click 'Add Comment' or equivalent action.</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>Application settings can be changed and applied successfully. UI themes update immediately. Default paths are honored. Language settings persist across restarts. Invalid input for settings is rejected with an appropriate error message.</t>
+          <t>The application displays an error or warning message (e.g., 'Comment cannot be empty', 'Please enter text to add a comment') and prevents the addition of an empty comment. The application remains stable.</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -1576,27 +1678,30 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>TC036</t>
+          <t>TC_COMMENTS_001_BOUNDARY_001</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Verify Search and Replace functionality for text within requirements and sections.</t>
+          <t>Verify application handles adding a very long comment to a requirement.</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>An opened document containing requirements with repeated text strings.</t>
+          <t>A document with requirements is open. A requirement is selected.</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>1. Use the 'Search' function to find an existing text string (e.g., 'user story'). 2. Verify all occurrences are found and highlighted. 3. Use the 'Replace' function to replace one occurrence of 'user story' with 'user requirement'. 4. Verify only that single occurrence is replaced. 5. Use 'Replace All' to replace all occurrences of 'user requirement' with 'feature'. 6. Verify all previous occurrences are replaced. 7. (Negative) Attempt to replace a non-existent string. 8. (Edge) Search/Replace with very long strings, special characters, and case-sensitive/insensitive options.</t>
+          <t>1. Select a requirement.
+2. Navigate to the 'Discussion' pane.
+3. Enter an extremely long text string (e.g., 4000+ characters) into the comment input field.
+4. Click 'Add Comment'.</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>The search function accurately finds and highlights occurrences. 'Replace' replaces a single instance. 'Replace All' replaces all instances. An appropriate message is displayed if the search string is not found for replace. Search and Replace handle long strings, special characters, and respect case sensitivity settings.</t>
+          <t>The very long comment is successfully added to the requirement. The application displays the full comment text without truncation or corruption. The UI (discussion pane) handles the display of the long text gracefully (e.g., with scrollbars if necessary). Performance for adding and viewing the comment remains acceptable. If there's a character limit, a clear error message should be displayed.</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -1608,123 +1713,140 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>TC037</t>
+          <t>TC_COMMENTS_001_SEC_001</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Verify basic keyboard navigation and accessibility for key UI elements.</t>
+          <t>Verify application sanitizes comment input to prevent XSS vulnerabilities.</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>An opened document.</t>
+          <t>A document with requirements is open. A requirement is selected.
+The 'Discussion' pane is visible. An XSS payload string (e.g., &lt;script&gt;alert('Comment XSS');&lt;/script&gt;) is available.</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>1. Use Tab key to navigate through main UI elements (menu bar, toolbar, TOC, requirements table, detail panes). 2. Use arrow keys to navigate within the requirements table (select different rows/columns). 3. Use Enter key to open a requirement for editing its description. 4. Use Escape key to close editing modes or dialogs. 5. (If supported) Use keyboard shortcuts for common actions (e.g., Ctrl+N for New, Ctrl+S for Save, Ctrl+Z for Undo).</t>
+          <t>1. Select a requirement.
+2. Navigate to the 'Discussion' pane.
+3. Enter the XSS payload into the comment input field.
+4. Click 'Add Comment'.
+5. Observe the displayed comment.</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>Users can navigate through main UI elements using the Tab key, with clear focus indication. Arrow keys allow navigation within tables. Enter key initiates editing or opens selected items. Escape key correctly cancels operations or closes UI elements. Keyboard shortcuts execute corresponding actions correctly.</t>
+          <t>The application sanitizes the comment input, stripping out or escaping any potentially malicious HTML/script tags. The XSS payload is NOT executed when the comment is displayed. The application remains secure and stable.</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>Low</t>
+          <t>High</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>TC038</t>
+          <t>TC_LINKS_CONFIG_001</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Verify context menu actions for requirements, sections, attachments, and links.</t>
+          <t>Verify user can successfully define a new traceability link type.</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>An opened document with requirements, sections, attachments, and links.</t>
+          <t>Application is launched and a document is open. User has permissions to configure link types.</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>1. Right-click on a requirement in the table. 2. Verify the context menu appears with relevant actions (e.g., Copy, Cut, Delete, Mark as Deleted, Comment, Attach File). 3. Select an action (e.g., 'Copy') and verify its effect. 4. Right-click on a section in the TOC or table. 5. Verify section-specific actions (e.g., Create Requirement, Create Section, Move Section). 6. Right-click on an attachment in the attachments pane. 7. Verify attachment-specific actions (e.g., Save As, Remove). 8. Right-click on a link in the links pane. 9. Verify link-specific actions (e.g., Remove Link, Go To Linked Item).</t>
+          <t>1. Go to 'Traceability Links Configuration' settings.
+2. Click 'Add New Link Type'.
+3. Set a unique and valid name for the link type (e.g., 'Implements').
+4. Set descriptive role names for the source (e.g., 'Implemented By') and target (e.g., 'Implements').
+5. Save the link type definition.
+6. Verify its availability.</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>Context menus appear correctly for all clickable elements. All actions available in the context menu are relevant to the selected item and execute successfully when chosen. Disabled actions (e.g., 'Permanently Remove' for non-deleted item) are greyed out.</t>
+          <t>A new link type is successfully defined with the specified name and role names. It is assigned a unique, immutable ID and becomes available for creating links between requirements. The link type is listed in the configuration settings. No errors are displayed.</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>High</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>TC039</t>
+          <t>TC_LINKS_CONFIG_001_NEG_001</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Verify Undo/Redo functionality for complex operations (e.g., Move Section, Import, Filter, Bulk Edit).</t>
+          <t>Verify application prevents defining a new link type with an empty or duplicate name/role names.</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>An opened document with a complex structure and data. The application has Undo/Redo capabilities.</t>
+          <t>Application is launched and a document is open.</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>1. Perform a 'Move Section' operation on a section with many sub-items. 2. Use 'Undo'. 3. Verify the section reverts to its original position. 4. Use 'Redo'. 5. Verify the section moves back. 6. Import a Word document (TC003). 7. Use 'Undo'. 8. Verify the imported requirements are removed. 9. Use 'Redo'. 10. Verify the requirements are re-imported. 11. Apply a complex filter. 12. Use 'Undo'. 13. Verify the filter is cleared. 14. Use 'Redo'. 15. Verify the filter is reapplied. 16. Perform a 'Replace All' operation (TC036). 17. Use 'Undo'. 18. Verify the text reverts.</t>
+          <t>1. Go to 'Traceability Links Configuration'.
+2. Attempt to add a new link type with an empty 'Name'.
+3. Attempt to add a new link type with a 'Name' that already exists.
+4. Attempt to add a new link type with empty 'Source Role' or 'Target Role' names.</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>The 'Undo' and 'Redo' actions successfully reverse and re-apply changes for complex operations such as moving sections, importing content, applying/clearing filters, and bulk edits. The UI updates correctly, reflecting the state before/after the operation.</t>
+          <t>In all cases, the application displays an error message (e.g., 'Name cannot be empty', 'Link type already exists', 'Role name cannot be empty') and prevents the creation of the invalid link type. The application remains stable.</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>High</t>
+          <t>Medium</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>TC040</t>
+          <t>TC_LINKS_MANAGEMENT_001</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Verify file compatibility: Opening documents created with older/newer application versions (if versioning is applicable).</t>
+          <t>Verify user can successfully create a directed traceability link between selected requirements.</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Application is running. Document files created with a previous major version ('OldVersion.req') and a future (not yet officially released, if simulated) version ('NewVersion.req') are available.</t>
+          <t>A document with at least two requirements (e.g., Req A and Req B) is open. A link type is defined and available (e.g., 'Implements').</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>1. Attempt to open 'OldVersion.req'. 2. Verify it opens correctly. 3. Make some changes and save. 4. Verify it saves in the current version's format (possibly with a warning about upgrade). 5. Attempt to open 'NewVersion.req'.</t>
+          <t>1. Select a source requirement (Req A).
+2. Select a target requirement (Req B).
+3. Initiate 'Create Traceability Link' action (e.g., context menu, toolbar button).
+4. Choose an existing link type (e.g., 'Implements').
+5. Confirm the link creation.</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>Documents from older versions open successfully, converting to the current format if necessary. A prompt or warning might inform the user of the version upgrade. Changes made to older version documents are saved in the current application version. Documents from newer versions should either open with a warning (if backward compatible) or display an error message indicating incompatibility (e.g., 'Document created with a newer version. Please update your application.'). The application should not crash.</t>
+          <t>A directed traceability link of the chosen type is successfully created between Req A and Req B. The link is immediately displayed in the 'Links' pane for both Req A (as an outgoing link) and Req B (as an incoming link), grouped by link type and showing the respective role names. The application remains stable, and no errors are displayed.</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -1736,27 +1858,29 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>TC041</t>
+          <t>TC_LINKS_MANAGEMENT_002</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Verify UI responsiveness during heavy operations (e.g., filtering a large document, importing large files).</t>
+          <t>Verify application prevents creating a traceability link with an invalid selection (e.g., linking a requirement to itself).</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>An opened large document (TC027) with complex data. A large import file (TC003).</t>
+          <t>A document with requirements is open. A link type is defined.</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>1. While a large document is open, apply a complex filter condition and observe UI responsiveness. 2. While a large document is open, scroll through the requirements table rapidly. 3. Initiate an import of a large Word/Excel file. 4. During the import process, attempt to interact with other UI elements (e.g., click menus, resize windows).</t>
+          <t>1. Select a single requirement (e.g., Req 1).
+2. Attempt to create a traceability link using only this single requirement as both source and target (if the UI allows such a selection).
+3. Attempt to create a link from a requirement to a non-existent requirement (if UI allows entering IDs).</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>The UI remains responsive during filtering operations; the filter is applied efficiently, and the display updates without significant delays or freezing. Rapid scrolling through a large document is smooth and without lag. During long-running operations like large imports, the UI should remain responsive, allowing users to interact with other elements or showing a progress indicator, without freezing the entire application.</t>
+          <t>The application either prevents the user from selecting the same requirement as both source and target (e.g., 'Self-linking is not allowed'), or displays an error message and aborts the creation. Similarly, it prevents linking to non-existent requirements. The application remains stable and no invalid links are created.</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -1768,27 +1892,28 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>TC042</t>
+          <t>TC_LINKS_MANAGEMENT_001_EDGE_001</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Verify error logging mechanism by triggering various error conditions.</t>
+          <t>Verify the display and performance when a single requirement has a very large number of incoming and outgoing links.</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Application is running. Access to application logs directory.</t>
+          <t>A document is open. A central 'hub' requirement (Req H) has been linked to/from hundreds or thousands of other requirements using various link types.</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>1. Trigger a 'File Not Found' error (TC022, step 3). 2. Trigger a 'Permission Denied' error (TC022, step 11). 3. Trigger a 'Corrupted File' error (TC022, step 5). 4. Trigger an XSS attack attempt (TC030). 5. Review the application log files.</t>
+          <t>1. Select the 'hub' requirement (Req H).
+2. Navigate to its 'Links' pane.</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>Appropriate error messages are displayed to the user. Detailed error information (e.g., timestamp, error type, affected module, stack trace if applicable) for each triggered error condition is recorded in the application log files. Sensitive information is not exposed in logs unless necessary for debugging and anonymized if production.</t>
+          <t>The 'Links' pane for Req H successfully displays all incoming and outgoing links. The UI remains responsive (e.g., scrolling, filtering links if available), and all link details (type, target/source requirement, role) are correctly presented. No performance degradation or crashes occur due to the large number of links.</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -1800,27 +1925,30 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>TC043</t>
+          <t>TC_FILTER_SEARCH_001</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Verify concurrent access/file locking behavior when opening a file already in use by another application.</t>
+          <t>Verify user can successfully filter requirements using a valid DNF (Disjunctive Normal Form) condition.</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Application is closed. A valid document file ('SharedDoc.req') is open and locked by another application (e.g., Notepad, Word) in an exclusive write mode.</t>
+          <t>A document with diverse requirements, sections, and custom attributes (including various data types) is open. Some requirements match the DNF condition, others do not.</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>1. Start the application. 2. Navigate to 'File' menu. 3. Select 'Open Document'. 4. Choose 'SharedDoc.req' and click 'Open'.</t>
+          <t>1. Access the filtering mechanism.
+2. Enter a valid DNF condition (e.g., (Priority = 'High' AND Status = 'Open') OR (Assignee = 'John Doe' AND Type = 'Functional')).
+3. Apply the filter.
+4. Verify the displayed requirements.</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>An appropriate error message is displayed, indicating that the file is locked, in use by another process, or cannot be accessed (e.g., 'File locked', 'Permission denied'). The application should not crash or corrupt the file. The file should remain readable by the other application.</t>
+          <t>Only requirements that precisely match the specified DNF condition are displayed in the requirements table. Requirements that do not match the condition are hidden. The filtered view is accurate according to the logical condition, and the application's responsiveness is maintained during filtering. A clear indication of an active filter is visible.</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -1832,27 +1960,29 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>TC044</t>
+          <t>TC_FILTER_SEARCH_001_NEG_001</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Verify handling of non-ASCII/Unicode characters in file paths and names.</t>
+          <t>Verify application handles applying a filter with invalid DNF syntax or non-existent attributes.</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Application is running. A document named with Unicode characters (e.g., 'ДокументСпецификации.req', '日本文書.req') exists. A folder with Unicode characters in its name exists (e.g., 'Мои Документы').</t>
+          <t>A document is open.</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>1. Navigate to 'File' menu. 2. Select 'Open Document'. 3. Choose a document with Unicode characters in its name. 4. Verify the document opens correctly. 5. Create a new document. 6. Select 'Save As'. 7. Choose a folder path with Unicode characters. 8. Give the document a name with Unicode characters and save it. 9. Verify the document is saved and can be re-opened.</t>
+          <t>1. Access the filtering mechanism.
+2. Enter an invalid DNF condition (e.g., unmatched parentheses, invalid operator, referencing a non-existent custom attribute, Priority = 'High' AND (Status).
+3. Attempt to apply the filter.</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>The application successfully opens documents with Unicode characters in their filenames and paths. Documents can be saved with Unicode characters in their filenames and to paths containing Unicode characters, and these documents can be re-opened correctly. No encoding issues or file access errors occur.</t>
+          <t>The application displays a clear error message indicating a syntax error, an invalid attribute reference, or an unparsable condition. The invalid filter is NOT applied, and the document view remains unchanged. The application remains stable.</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -1864,32 +1994,483 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>TC045</t>
+          <t>TC_FILTER_SEARCH_001_EDGE_001</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Verify document corruption handling and recovery upon unexpected application termination during a save operation.</t>
+          <t>Verify application handles applying a filter that matches no requirements.</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Application is running. An existing document ('CriticalDoc.req') is available. A mechanism to simulate application termination (e.g., Task Manager 'End Task').</t>
+          <t>A document with requirements is open.</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>1. Open 'CriticalDoc.req'. 2. Make significant changes (e.g., add/delete multiple requirements, sections, attachments). 3. Initiate a 'Save' operation. 4. Immediately after initiating save, force-quit the application (e.g., 'End Task'). 5. Restart the application. 6. Attempt to open 'CriticalDoc.req'.</t>
+          <t>1. Access the filtering mechanism.
+2. Enter a valid DNF condition that is known to match no existing requirements (e.g., (Priority = 'NonExistent' AND Status = 'Invalid')).
+3. Apply the filter.</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>Upon restart, the application attempts to open 'CriticalDoc.req'. If the file was corrupted during the interrupted save, the application should either: a) open a valid previous version/backup, b) display an error message and offer recovery options (if available), or c) display an error that the file is corrupted. The application should not crash, and ideally, data loss should be minimized (e.g., only changes from the last save lost, or a partial recovery).</t>
+          <t>The filter is successfully applied, and the requirements table displays an empty set or a message indicating 'No requirements match the filter criteria'. No errors are displayed, and the application remains stable.</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
+          <t>Low</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>TC_FILTER_SEARCH_002</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Verify user can search for keywords and navigate through matched requirements.</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>A document with requirements is open, and some requirements contain specific keywords (e.g., 'Login', 'Security') in their descriptions or other visible fields.</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>1. Activate the search function (e.g., Ctrl+F, search bar).
+2. Enter a keyword (e.g., 'Login').
+3. Use 'Next Match' and 'Previous Match' navigation buttons/controls.
+4. Change the search keyword.</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>The application highlights all occurrences of the keyword within the visible document content. Users can successfully navigate between matched requirements using the 'Next' and 'Previous' buttons. The view automatically scrolls to and focuses on the current matched requirement. The total count of matches is displayed. Changing keywords updates the search results accurately. The search function is case-insensitive by default or offers a case-sensitive option.</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
           <t>High</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>TC_FILTER_SEARCH_002_NEG_001</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Verify application handles searching for a keyword that does not exist in the document.</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>A document with requirements is open.</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>1. Activate the search function.
+2. Enter a keyword that is known to not exist anywhere in the document (e.g., 'xyzzy').
+3. Press Enter or activate search.</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>The application indicates that no matches were found (e.g., '0 of 0', 'No results found'). No requirements are highlighted, and no errors are displayed. The application remains stable.</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>TC_FILTER_SEARCH_002_EDGE_001</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Verify application handles searching for very long keywords or keywords with special characters.</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>A document is open, potentially containing very long words or words with special characters.</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>1. Activate the search function.
+2. Enter a very long keyword (e.g., a full sentence).
+3. Enter a keyword containing special characters (e.g., !@#$%^&amp;*()).
+4. Observe search results and navigation.</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>The search function correctly identifies and highlights matches for very long keywords and keywords containing special characters, assuming these characters are part of the searchable content. Performance remains acceptable, and the application remains stable. Special character handling is consistent.</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>TC_HISTORY_001</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Verify the History pane displays all relevant changes for a selected requirement, ordered by date and time.</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>A document is open. A specific requirement has undergone multiple types of changes (e.g., description edited, custom attribute value changed, comment added, link created/deleted, section moved). The 'History' pane is visible.</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>1. Select the requirement with multiple changes.
+2. Observe the 'History' pane.
+3. Verify the details of each change.</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>The 'History' pane displays a comprehensive list of all tracked changes made to the selected requirement. Each change entry includes: the author (user who made the change), the exact date and time of the change, and a clear, descriptive summary of the change (e.g., 'Description updated', 'Priority changed from Low to High', 'Comment added', 'Link 'Implements' to Req-002 created'). The entries are consistently ordered chronologically (e.g., newest first).</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>TC_HISTORY_001_EDGE_001</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Verify history for a newly created requirement.</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>A document is open.</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>1. Create a new requirement.
+2. Immediately select the new requirement.
+3. Observe the 'History' pane.</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>The 'History' pane should display only one entry: the 'Requirement created' event, including the author, date, and time. There should be no other change entries, and the pane should indicate no further history. No errors are displayed.</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>TC_HISTORY_001_BOUNDARY_001</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Verify performance and stability of the History pane for a requirement with an extremely large number of changes.</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>A requirement exists that has been subjected to thousands of modifications (e.g., script-driven frequent attribute updates, many comments).</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>1. Select the requirement with an extremely large change history.
+2. Navigate to its 'History' pane.
+3. Scroll through the history entries.</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>The 'History' pane loads and displays the large number of change entries within an acceptable time frame. Scrolling through the history is fluid and responsive. The application remains stable, and there is no significant performance degradation or crash. If pagination is implemented, it functions correctly.</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>TC_APP_LIFECYCLE_001</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Verify the application automatically persists document changes and restores its state upon restart.</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Application is launched. Auto-save/auto-persistence feature is enabled (which is implicit for 'persists changes').</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>1. Create a new document and add several requirements and sections.
+2. Add some comments and traceability links.
+3. Modify some custom attribute values.
+4. Close the application gracefully without explicitly clicking 'Save' (relying on auto-persistence).
+5. Relaunch the application.</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>Upon relaunch, the application successfully restores the document to its last known state, including all added requirements, sections, comments, links, and modified attribute values. No data loss occurs from the last auto-saved state. The document view is identical to before closure. The application launches successfully and remains stable.</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>TC_APP_LIFECYCLE_001_NEG_001</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Verify behavior if application crashes or is forcefully terminated during active work (simulated crash).</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Application is launched and a new document is open with unsaved changes. Auto-save is enabled.</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>1. Create a new document and add some content (requirements, sections, comments).
+2. Forcefully terminate the application process (e.g., using Task Manager 'End Task', 'kill' command) without graceful shutdown.
+3. Relaunch the application.</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>Upon relaunch, the application should attempt to recover the document to its last auto-saved state, or prompt the user to recover. Critical data loss should be minimized, and the application should not crash on startup. A clear message about recovery status should be shown if applicable. The application remains stable.</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>TC_BOUNDARY_001</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Verify performance and stability when opening a document with 10,000 objects (requirements/sections).</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>A pre-existing document file containing exactly 10,000 requirements and/or sections is available.</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>1. Launch the application.
+2. Open the document with 10,000 objects.
+3. Perform basic interactions: scroll through the TOC and requirements table, select individual requirements, open detail panes.</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>The document opens successfully within an acceptable time frame (e.g., less than 15-20 seconds for initial load). The application remains responsive during basic interactions; scrolling is smooth, selecting items is quick, and the detail pane loads promptly. All 10,000 objects are displayed correctly without crashing, significant performance degradation, or UI freezes.</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>TC_BOUNDARY_002</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Verify application handles a document with maximum allowed nesting depth for sections/requirements.</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>A document with a deep hierarchical structure (e.g., 10+ levels of nested sections and requirements) is available.</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>1. Open the deeply nested document.
+2. Expand/collapse various levels in the TOC.
+3. Scroll through the requirements table.</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>The application correctly displays the entire hierarchical structure without UI glitches, performance issues, or crashes. Expanding and collapsing nodes is responsive. All requirements and sections at all depths are accessible and editable. If there's an explicit maximum nesting depth, verify that the application prevents exceeding it gracefully.</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>TC_BOUNDARY_003</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Verify application handles a document where all requirements utilize the maximum number of custom attributes (if limited).</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>A document is open where each requirement has been assigned values for the maximum allowed number of custom attributes (e.g., 20+ custom attributes per requirement).</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>1. Open the document.
+2. Observe the requirements table (which might display many columns).
+3. Select a requirement and view its detail pane with all custom attributes.
+4. Attempt to edit some custom attribute values.</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>The application displays all custom attribute columns and values correctly without visual overflow or performance issues. Editing values is responsive. The application remains stable, and no data corruption occurs due to the high density of attributes.</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>TC_EDGE_001</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Verify application handles operations like filtering, searching, or exporting when the document is entirely empty.</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>A new, empty document is open (contains no sections or requirements).</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>1. Attempt to apply a filter condition.
+2. Attempt to perform a search for any keyword.
+3. Attempt to export the document view to HTML or CSV.
+4. Attempt to print the document.</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>The application handles these operations gracefully without errors or crashes. Filtering and searching yield no results (as expected) with an appropriate 'no results' message. Exporting an empty document results in an empty or minimal HTML/CSV file without errors. Printing an empty document produces an empty page or a document title. The application remains stable.</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>TC_EDGE_002</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>Verify application handles extremely long document names, section names, and requirement descriptions.</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>A document exists with: an extremely long document name, a section name of maximum allowed length, and a requirement description of maximum allowed length (if not already covered by TC_EDIT_STRUCT_001_BOUNDARY_001).</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>1. Open the document.
+2. Observe the document name in the title bar/tabs.
+3. Observe the long section name in the TOC.
+4. Select the requirement with the very long description.</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>The application displays these long names and descriptions correctly, possibly truncating with ellipses if necessary in UI elements but retaining full data in the backend. No UI overflow, rendering issues, or performance degradation occurs. The application remains stable and functional.</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>Low</t>
         </is>
       </c>
     </row>

</xml_diff>